<commit_message>
Task #2, practice, modified
</commit_message>
<xml_diff>
--- a/2_Theory_of_testing/ДЗ 2 Горшков Дмитрий.xlsx
+++ b/2_Theory_of_testing/ДЗ 2 Горшков Дмитрий.xlsx
@@ -18,9 +18,272 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="86">
+  <si>
+    <t>Название (Summary):</t>
+  </si>
+  <si>
+    <t>Критичность/Серьезность (Severity):</t>
+  </si>
+  <si>
+    <t>Описание( Description):</t>
+  </si>
+  <si>
+    <t>Шаги (Steps to reproduce):</t>
+  </si>
+  <si>
+    <t>Фактический результат (Actual result):</t>
+  </si>
+  <si>
+    <t>Ожидаемый результат (Expected result):</t>
+  </si>
+  <si>
+    <t>Ссылка на вложение (Attachments)</t>
+  </si>
+  <si>
+    <t>Ошибка (падение) при незаполненных полях</t>
+  </si>
+  <si>
+    <t>Блокер (Blocker)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Полная версия сайта; Мобильная версия сайта. </t>
+  </si>
+  <si>
+    <t>1. Перейти на шаг2</t>
+  </si>
+  <si>
+    <t>Появляется экран с ошибкой "Что-то пошло не так". При нажатии на кнопку Назад переход на https://alfabank.ru/</t>
+  </si>
+  <si>
+    <t>Поле Район подсвечивается красным как обязательное к заполнению. Переход к следующему шагу. Отсутсвие ошибок.</t>
+  </si>
+  <si>
+    <t>https://gyazo.com/83e08ec4138b3ed5cb040a35640b1442</t>
+  </si>
+  <si>
+    <t>Анкета падает, если на втором шаге оставить поля Район и корпус пустыми и отправить форму на следующий шаг</t>
+  </si>
+  <si>
+    <t>2. Заполнить все поля</t>
+  </si>
+  <si>
+    <t>3. Поля Район и корпус в Адресе постоянной регистрации оставить пустыми</t>
+  </si>
+  <si>
+    <t>4. Нажать на кнопку Продолжить</t>
+  </si>
+  <si>
+    <t>Слишком короткий таймаут</t>
+  </si>
+  <si>
+    <t>Крититичекая (Critical)</t>
+  </si>
+  <si>
+    <t>1. Перейти на страницу анкеты: https://testjmb.alfabank.ru/land/alfaform-dc-new/step1?cardId=DS&amp;packetId=N01&amp;platformId=test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Появляется поп-ап с уведомлением об истечении текущей сессии и невозможностью вернуться к заполнению </t>
+  </si>
+  <si>
+    <t>Таймаут минимум 15 минут. По истечение времени показывать поп-ап скнопкой Продолжить заполнение https://gyazo.com/a91f1fe74e40052ca44abcb083aa5e5d</t>
+  </si>
+  <si>
+    <t>https://gyazo.com/46875b4073da52d429b9aa01bc2b7ddf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 минут не хватает, чтобы прочитать оферту. Нельзя закрыть поп-ап, чтобы вернуться к заполнению анкеты. Ранее введенные данные не сохраняются. Приходится вводить все заново. </t>
+  </si>
+  <si>
+    <t>2. Заполнить поля</t>
+  </si>
+  <si>
+    <t>3. Открыть оферту: "Нажимая кнопку «Продолжить», я подтверждаю, что ознакомлен и согласен с условиями направления заявления"</t>
+  </si>
+  <si>
+    <t>4. Медленно листать оферту(~ 3 минуты)</t>
+  </si>
+  <si>
+    <t>Не валидируются поля в Адресе постоянной регистрации</t>
+  </si>
+  <si>
+    <t>Средняя (Medium)</t>
+  </si>
+  <si>
+    <t>Мобильная версия сайта, Safari, ios 11.2.2</t>
+  </si>
+  <si>
+    <t>1. Перейти к шагу 2 из 4</t>
+  </si>
+  <si>
+    <t>Допускается введение рандомных последовательностей букв цифр и спецсимволов в поля адреса. Возможен переход на следующий шаг.</t>
+  </si>
+  <si>
+    <t>При введении рандомных последовательностей символов в поля Район, Населенный пункт, Улица, Индекс не срабатывает распознавание, и следовательно, поле подствечивается красным. В полях дом, корпус, квартира разрешить только ввод цифр, букв, / (например 142а/80). Остальные спецсимволы запретить.</t>
+  </si>
+  <si>
+    <t>https://gyazo.com/a697545d8a7db717a3b16b7393fa2d40</t>
+  </si>
+  <si>
+    <t>На втором шаге для адреса прописки и фактического проживания поля можно заполнить рандомными символами.</t>
+  </si>
+  <si>
+    <t>2. Заполнить адрес постоянной регистрации</t>
+  </si>
+  <si>
+    <t>3. Начать вводить название существующей улицы</t>
+  </si>
+  <si>
+    <t>4. Перейти к заполнению индекса. Начать вводить индекс</t>
+  </si>
+  <si>
+    <t>5. После заполнения всех полей нажать на кнопку Продолжить</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Таймер сбрасывается при повторном изменениии номера телефона </t>
+  </si>
+  <si>
+    <t>1. Дойти до 4 шага заполнения анкеты. Вырать регион и Способ получения карты. Нажать прододжить.</t>
+  </si>
+  <si>
+    <t>Кнопка "Изменить номер телефона"  кликабельна  во время отсчета 1 минуты с момента последней отправки кода</t>
+  </si>
+  <si>
+    <t>Кнопка "Изменить номер телефона" не кликабельна, пока идет отсчет 1 минуты.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://gyazo.com/94f66136552d35dcd16fdd3e48c50c6a  </t>
+  </si>
+  <si>
+    <t>Можно менять номер телефона до истечения 1 минуты. Т.о. происходит обход таймера, высылаются дополнительные смс =&gt; дополнительные расходы, а так же возможная для клиента путаница в кодах ввиду задержки отправления смс.</t>
+  </si>
+  <si>
+    <t>2. В поп-апе введения кода нажать кнопку "Изменить номер телефона."</t>
+  </si>
+  <si>
+    <t>3. Ввести новый номер телефона</t>
+  </si>
+  <si>
+    <t>4. Нажать кнопку Изменить</t>
+  </si>
+  <si>
+    <t>5. Повторить шаги 2-3 еще 4 раза</t>
+  </si>
+  <si>
+    <t>В поле "Серия старого паспорта" можно вводить буквы и символы</t>
+  </si>
+  <si>
+    <t>Полная версия сайта; Мобильная версия сайта.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Перейти на шаг 2 </t>
+  </si>
+  <si>
+    <t>Допусткается ввод цифр, символов и букв</t>
+  </si>
+  <si>
+    <t>Допускается ввод только цифр</t>
+  </si>
+  <si>
+    <t>https://gyazo.com/5aad3c8d33b4711be81a3a07b3c24499</t>
+  </si>
+  <si>
+    <t>2. Выбрать радиобаттон Да в графе Вы меняли паспорт?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3. Ввести в поле серии буквы и симполы </t>
+  </si>
+  <si>
+    <t>Отсутсвует счетчик попыток получения кода из смс</t>
+  </si>
+  <si>
+    <t>Появляется экран "Вы превысили количество попыток получения кода". Счетчик попыток отсутсвует.</t>
+  </si>
+  <si>
+    <t>На поп-апе с вводом кода из смс есть счетчик попыток.</t>
+  </si>
+  <si>
+    <t>https://gyazo.com/ddbf8b13fda33438cb90629a796eb8b6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Нигде в анкете не указано максимальное число попыток получения кода. </t>
+  </si>
+  <si>
+    <t>2. Заполнить необходимые поля, дойти до 4 шага</t>
+  </si>
+  <si>
+    <t>3. В поп-апе введения кода нажать кнопку "Изменить номер телефона."</t>
+  </si>
+  <si>
+    <t>4. Ввести номер телефона</t>
+  </si>
+  <si>
+    <t>5. Проделать шаги 3-4 несколько раз</t>
+  </si>
+  <si>
+    <t>Не распознаются поля в Адресе постоянной регистрации</t>
+  </si>
+  <si>
+    <t>Низкая (Low)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Улица, район, населенный пункт не распознаются. Проверка индекса осуществляется только на длинну ввода </t>
+  </si>
+  <si>
+    <t>При введении улицы, района, населенного пункта -- автозаполнение из базы. Если такой улицы, района, населенного пункта нет в базе, подсвечивать поле красным. При введении индекса включается автозаполнение из базы индексов. Если индекс введен ошибочно, подсвечивать поле красным.</t>
+  </si>
+  <si>
+    <t>https://gyazo.com/3fc985a575a4ea84e598637a4ad1c232</t>
+  </si>
+  <si>
+    <t>На втором шаге для адреса прописки и фактического проживания нет автозаполнения индекса и улицы</t>
+  </si>
+  <si>
+    <t>3. Начать вводить название существующей улицы, района, населенного пункта</t>
+  </si>
+  <si>
+    <t>Не работает плавный скроллинг в оферте</t>
+  </si>
+  <si>
+    <t>Резкий скроллинг</t>
+  </si>
+  <si>
+    <t>Плавный скроллинг: пока юзер держит палец на экране.</t>
+  </si>
+  <si>
+    <t>*здесь могла бы быть видеозапись экрана айфона, но баг минорный, поэтому ее нет*</t>
+  </si>
+  <si>
+    <t>Резкое пролистывание оферты.</t>
+  </si>
+  <si>
+    <t>2. Открыть оферту: Нажимая кнопку «Продолжить», я подтверждаю, что ознакомлен и согласен с условиями направления заявления</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3. Медленно листать оферту </t>
+  </si>
+  <si>
+    <t>Скроллбар пропадает при пролистывании офреты</t>
+  </si>
+  <si>
+    <t>Скроллбар появляется только в начале и в конце страницы, пока юзер листает оферту, скорллбар отсутсвует.</t>
+  </si>
+  <si>
+    <t>Скроллбар отображается на протяжении пролистывания от начала и до конца оферты</t>
+  </si>
+  <si>
+    <t>https://gyazo.com/c956818bd4d20e475a28676dd3b69f78  https://gyazo.com/3cd92b187583eb018197167533394eaf</t>
+  </si>
+  <si>
+    <t>Нет скроллбара по время листания. При чтении не понятно, когда закончится документ.</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -28,16 +291,109 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCFE2F3"/>
+        <bgColor rgb="FFCFE2F3"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF4CCCC"/>
+        <bgColor rgb="FFF4CCCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFF2CC"/>
+        <bgColor rgb="FFFFF2CC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9EAD3"/>
+        <bgColor rgb="FFD9EAD3"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEAD1DC"/>
+        <bgColor rgb="FFEAD1DC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9D2E9"/>
+        <bgColor rgb="FFD9D2E9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE6B8AF"/>
+        <bgColor rgb="FFE6B8AF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF3F3F3"/>
+        <bgColor rgb="FFF3F3F3"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCC0000"/>
+        <bgColor rgb="FFCC0000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE06666"/>
+        <bgColor rgb="FFE06666"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFD966"/>
+        <bgColor rgb="FFFFD966"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF6AA84F"/>
+        <bgColor rgb="FF6AA84F"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -45,15 +401,249 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -69,9 +659,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -109,12 +699,12 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="Yu Gothic Light"/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
         <a:font script="Hans" typeface="等线 Light"/>
         <a:font script="Hant" typeface="新細明體"/>
@@ -149,7 +739,7 @@
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="Yu Gothic"/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
         <a:font script="Hans" typeface="等线"/>
         <a:font script="Hant" typeface="新細明體"/>
@@ -181,7 +771,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -331,12 +921,635 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16:C19"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26.7109375" style="8" customWidth="1"/>
+    <col min="2" max="2" width="17.5703125" style="8" customWidth="1"/>
+    <col min="3" max="3" width="26.85546875" style="8" customWidth="1"/>
+    <col min="4" max="4" width="65.42578125" style="8" customWidth="1"/>
+    <col min="5" max="5" width="24" style="8" customWidth="1"/>
+    <col min="6" max="6" width="25" style="8" customWidth="1"/>
+    <col min="7" max="7" width="31.85546875" style="8" customWidth="1"/>
+    <col min="8" max="16384" width="14.42578125" style="8"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="15" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="16"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="17"/>
+    </row>
+    <row r="4" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A4" s="16"/>
+      <c r="B4" s="17"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="17"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="20"/>
+      <c r="B5" s="21"/>
+      <c r="C5" s="20"/>
+      <c r="D5" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="21"/>
+      <c r="F5" s="21"/>
+      <c r="G5" s="21"/>
+    </row>
+    <row r="6" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A6" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="G6" s="26" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="16"/>
+      <c r="B7" s="16"/>
+      <c r="C7" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="E7" s="16"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="16"/>
+    </row>
+    <row r="8" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A8" s="16"/>
+      <c r="B8" s="16"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" s="16"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="16"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="20"/>
+      <c r="B9" s="20"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="E9" s="20"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="20"/>
+    </row>
+    <row r="10" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A10" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="G10" s="29" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="16"/>
+      <c r="B11" s="16"/>
+      <c r="C11" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="E11" s="16"/>
+      <c r="F11" s="16"/>
+      <c r="G11" s="16"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="16"/>
+      <c r="B12" s="16"/>
+      <c r="C12" s="16"/>
+      <c r="D12" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="E12" s="16"/>
+      <c r="F12" s="16"/>
+      <c r="G12" s="16"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="16"/>
+      <c r="B13" s="16"/>
+      <c r="C13" s="16"/>
+      <c r="D13" s="30" t="s">
+        <v>38</v>
+      </c>
+      <c r="E13" s="16"/>
+      <c r="F13" s="16"/>
+      <c r="G13" s="16"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="20"/>
+      <c r="B14" s="20"/>
+      <c r="C14" s="20"/>
+      <c r="D14" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="E14" s="20"/>
+      <c r="F14" s="20"/>
+      <c r="G14" s="20"/>
+    </row>
+    <row r="15" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A15" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="B15" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="D15" s="34" t="s">
+        <v>41</v>
+      </c>
+      <c r="E15" s="35" t="s">
+        <v>42</v>
+      </c>
+      <c r="F15" s="35" t="s">
+        <v>43</v>
+      </c>
+      <c r="G15" s="36" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="16"/>
+      <c r="B16" s="17"/>
+      <c r="C16" s="31" t="s">
+        <v>45</v>
+      </c>
+      <c r="D16" s="34" t="s">
+        <v>46</v>
+      </c>
+      <c r="E16" s="17"/>
+      <c r="F16" s="17"/>
+      <c r="G16" s="17"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="16"/>
+      <c r="B17" s="17"/>
+      <c r="C17" s="16"/>
+      <c r="D17" s="34" t="s">
+        <v>47</v>
+      </c>
+      <c r="E17" s="17"/>
+      <c r="F17" s="17"/>
+      <c r="G17" s="17"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="16"/>
+      <c r="B18" s="17"/>
+      <c r="C18" s="16"/>
+      <c r="D18" s="34" t="s">
+        <v>48</v>
+      </c>
+      <c r="E18" s="17"/>
+      <c r="F18" s="17"/>
+      <c r="G18" s="17"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="16"/>
+      <c r="B19" s="17"/>
+      <c r="C19" s="20"/>
+      <c r="D19" s="34" t="s">
+        <v>49</v>
+      </c>
+      <c r="E19" s="21"/>
+      <c r="F19" s="21"/>
+      <c r="G19" s="21"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="B20" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="C20" s="37" t="s">
+        <v>51</v>
+      </c>
+      <c r="D20" s="38" t="s">
+        <v>52</v>
+      </c>
+      <c r="E20" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="F20" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="G20" s="15" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="16"/>
+      <c r="B21" s="17"/>
+      <c r="C21" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D21" s="39" t="s">
+        <v>56</v>
+      </c>
+      <c r="E21" s="17"/>
+      <c r="F21" s="17"/>
+      <c r="G21" s="17"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="16"/>
+      <c r="B22" s="17"/>
+      <c r="C22" s="20"/>
+      <c r="D22" s="39" t="s">
+        <v>57</v>
+      </c>
+      <c r="E22" s="21"/>
+      <c r="F22" s="21"/>
+      <c r="G22" s="21"/>
+    </row>
+    <row r="23" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A23" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="B23" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="C23" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="D23" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="E23" s="40" t="s">
+        <v>59</v>
+      </c>
+      <c r="F23" s="40" t="s">
+        <v>60</v>
+      </c>
+      <c r="G23" s="41" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="16"/>
+      <c r="B24" s="17"/>
+      <c r="C24" s="27" t="s">
+        <v>62</v>
+      </c>
+      <c r="D24" s="25" t="s">
+        <v>63</v>
+      </c>
+      <c r="E24" s="17"/>
+      <c r="F24" s="17"/>
+      <c r="G24" s="17"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="16"/>
+      <c r="B25" s="17"/>
+      <c r="C25" s="16"/>
+      <c r="D25" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="E25" s="17"/>
+      <c r="F25" s="17"/>
+      <c r="G25" s="17"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="16"/>
+      <c r="B26" s="17"/>
+      <c r="C26" s="16"/>
+      <c r="D26" s="24" t="s">
+        <v>65</v>
+      </c>
+      <c r="E26" s="17"/>
+      <c r="F26" s="17"/>
+      <c r="G26" s="17"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="20"/>
+      <c r="B27" s="21"/>
+      <c r="C27" s="20"/>
+      <c r="D27" s="24" t="s">
+        <v>66</v>
+      </c>
+      <c r="E27" s="21"/>
+      <c r="F27" s="21"/>
+      <c r="G27" s="21"/>
+    </row>
+    <row r="28" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A28" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="B28" s="43" t="s">
+        <v>68</v>
+      </c>
+      <c r="C28" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D28" s="44" t="s">
+        <v>31</v>
+      </c>
+      <c r="E28" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="F28" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="G28" s="15" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="16"/>
+      <c r="B29" s="17"/>
+      <c r="C29" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="D29" s="38" t="s">
+        <v>36</v>
+      </c>
+      <c r="E29" s="17"/>
+      <c r="F29" s="17"/>
+      <c r="G29" s="17"/>
+    </row>
+    <row r="30" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A30" s="16"/>
+      <c r="B30" s="17"/>
+      <c r="C30" s="16"/>
+      <c r="D30" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="E30" s="17"/>
+      <c r="F30" s="17"/>
+      <c r="G30" s="17"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="20"/>
+      <c r="B31" s="21"/>
+      <c r="C31" s="20"/>
+      <c r="D31" s="30" t="s">
+        <v>38</v>
+      </c>
+      <c r="E31" s="21"/>
+      <c r="F31" s="21"/>
+      <c r="G31" s="21"/>
+    </row>
+    <row r="32" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A32" s="45" t="s">
+        <v>74</v>
+      </c>
+      <c r="B32" s="46" t="s">
+        <v>68</v>
+      </c>
+      <c r="C32" s="47" t="s">
+        <v>30</v>
+      </c>
+      <c r="D32" s="48" t="s">
+        <v>20</v>
+      </c>
+      <c r="E32" s="49" t="s">
+        <v>75</v>
+      </c>
+      <c r="F32" s="49" t="s">
+        <v>76</v>
+      </c>
+      <c r="G32" s="49" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A33" s="16"/>
+      <c r="B33" s="17"/>
+      <c r="C33" s="45" t="s">
+        <v>78</v>
+      </c>
+      <c r="D33" s="48" t="s">
+        <v>79</v>
+      </c>
+      <c r="E33" s="17"/>
+      <c r="F33" s="17"/>
+      <c r="G33" s="17"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="20"/>
+      <c r="B34" s="21"/>
+      <c r="C34" s="20"/>
+      <c r="D34" s="48" t="s">
+        <v>80</v>
+      </c>
+      <c r="E34" s="21"/>
+      <c r="F34" s="21"/>
+      <c r="G34" s="21"/>
+    </row>
+    <row r="35" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A35" s="50" t="s">
+        <v>81</v>
+      </c>
+      <c r="B35" s="46" t="s">
+        <v>68</v>
+      </c>
+      <c r="C35" s="51" t="s">
+        <v>30</v>
+      </c>
+      <c r="D35" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="E35" s="52" t="s">
+        <v>82</v>
+      </c>
+      <c r="F35" s="52" t="s">
+        <v>83</v>
+      </c>
+      <c r="G35" s="52" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A36" s="16"/>
+      <c r="B36" s="17"/>
+      <c r="C36" s="50" t="s">
+        <v>85</v>
+      </c>
+      <c r="D36" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="E36" s="17"/>
+      <c r="F36" s="17"/>
+      <c r="G36" s="17"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="20"/>
+      <c r="B37" s="21"/>
+      <c r="C37" s="20"/>
+      <c r="D37" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="E37" s="21"/>
+      <c r="F37" s="21"/>
+      <c r="G37" s="21"/>
+    </row>
+  </sheetData>
+  <mergeCells count="54">
+    <mergeCell ref="A35:A37"/>
+    <mergeCell ref="B35:B37"/>
+    <mergeCell ref="E35:E37"/>
+    <mergeCell ref="F35:F37"/>
+    <mergeCell ref="G35:G37"/>
+    <mergeCell ref="C36:C37"/>
+    <mergeCell ref="A32:A34"/>
+    <mergeCell ref="B32:B34"/>
+    <mergeCell ref="E32:E34"/>
+    <mergeCell ref="F32:F34"/>
+    <mergeCell ref="G32:G34"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="A28:A31"/>
+    <mergeCell ref="B28:B31"/>
+    <mergeCell ref="E28:E31"/>
+    <mergeCell ref="F28:F31"/>
+    <mergeCell ref="G28:G31"/>
+    <mergeCell ref="C29:C31"/>
+    <mergeCell ref="A23:A27"/>
+    <mergeCell ref="B23:B27"/>
+    <mergeCell ref="E23:E27"/>
+    <mergeCell ref="F23:F27"/>
+    <mergeCell ref="G23:G27"/>
+    <mergeCell ref="C24:C27"/>
+    <mergeCell ref="A20:A22"/>
+    <mergeCell ref="B20:B22"/>
+    <mergeCell ref="E20:E22"/>
+    <mergeCell ref="F20:F22"/>
+    <mergeCell ref="G20:G22"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="A15:A19"/>
+    <mergeCell ref="B15:B19"/>
+    <mergeCell ref="E15:E19"/>
+    <mergeCell ref="F15:F19"/>
+    <mergeCell ref="G15:G19"/>
+    <mergeCell ref="C16:C19"/>
+    <mergeCell ref="A10:A14"/>
+    <mergeCell ref="B10:B14"/>
+    <mergeCell ref="E10:E14"/>
+    <mergeCell ref="F10:F14"/>
+    <mergeCell ref="G10:G14"/>
+    <mergeCell ref="C11:C14"/>
+    <mergeCell ref="A6:A9"/>
+    <mergeCell ref="B6:B9"/>
+    <mergeCell ref="E6:E9"/>
+    <mergeCell ref="F6:F9"/>
+    <mergeCell ref="G6:G9"/>
+    <mergeCell ref="C7:C9"/>
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="E2:E5"/>
+    <mergeCell ref="F2:F5"/>
+    <mergeCell ref="G2:G5"/>
+    <mergeCell ref="C3:C5"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="G2" r:id="rId1"/>
+    <hyperlink ref="G6" r:id="rId2"/>
+    <hyperlink ref="G10" r:id="rId3"/>
+    <hyperlink ref="G15" r:id="rId4"/>
+    <hyperlink ref="G20" r:id="rId5"/>
+    <hyperlink ref="G23" r:id="rId6"/>
+    <hyperlink ref="G28" r:id="rId7"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>